<commit_message>
La prevalencia importa en la práctica
</commit_message>
<xml_diff>
--- a/data/Matriz_Confusion.xlsx
+++ b/data/Matriz_Confusion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Wsoft\Documents\Ciencia de Datos\Proyectos\Publicaciones\MachineLearning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60849029-6D61-4805-8B66-63FD73452A0C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592D7DC0-8E53-4ADF-981C-A459E0ACB165}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9465" xr2:uid="{4119D02A-E20D-4628-AAD2-606E385A218D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>A mesure of</t>
   </si>

</xml_diff>